<commit_message>
Updated agent files and app
</commit_message>
<xml_diff>
--- a/project_404/data_collection/~data_documentation/variable_names.xlsx
+++ b/project_404/data_collection/~data_documentation/variable_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gmitchjr\Academic\CAPP_122\git-Planet-Status-Code-404\Final-Project\project_404\data_collection\~data_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21280574-BC41-4F05-B9A5-27F8C0DCA13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BED44C1D-3019-4FA0-A553-86537063B813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="400">
   <si>
     <t>JSON_Variable</t>
   </si>
@@ -787,57 +787,6 @@
   </si>
   <si>
     <t>Percent of population speaking Non English languages at home</t>
-  </si>
-  <si>
-    <t>demographics.P_NHWHITE</t>
-  </si>
-  <si>
-    <t>Percent of Non-Hispanic Whites</t>
-  </si>
-  <si>
-    <t>Breakdown by Race</t>
-  </si>
-  <si>
-    <t>demographics.P_NHBLACK</t>
-  </si>
-  <si>
-    <t>Percent of Non-Hispanic Blacks</t>
-  </si>
-  <si>
-    <t>demographics.P_NHASIAN</t>
-  </si>
-  <si>
-    <t>Percent of Non-Hispanic Asians</t>
-  </si>
-  <si>
-    <t>demographics.P_HISP</t>
-  </si>
-  <si>
-    <t>Percent of Hispanics</t>
-  </si>
-  <si>
-    <t>demographics.P_NHAMERIND</t>
-  </si>
-  <si>
-    <t>Percent of Non-Hispanic American Indians</t>
-  </si>
-  <si>
-    <t>demographics.P_NHHAWPAC</t>
-  </si>
-  <si>
-    <t>Percent of Non-Hispanic Hawaiian/Pacific</t>
-  </si>
-  <si>
-    <t>demographics.P_NHOTHER_RACE</t>
-  </si>
-  <si>
-    <t>Percent of Non-Hispanic Other Race</t>
-  </si>
-  <si>
-    <t>demographics.P_NHTWOMORE</t>
-  </si>
-  <si>
-    <t>Percent of Two or More Non-Hispanic Races</t>
   </si>
   <si>
     <t>demographics.P_AGE_LT5</t>
@@ -1569,13 +1518,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9A37E71-F706-4ADD-A9BB-BDC00341A1C5}" name="Table1" displayName="Table1" ref="A1:D63" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D63" xr:uid="{B9A37E71-F706-4ADD-A9BB-BDC00341A1C5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9A37E71-F706-4ADD-A9BB-BDC00341A1C5}" name="Table1" displayName="Table1" ref="A1:D55" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D55" xr:uid="{B9A37E71-F706-4ADD-A9BB-BDC00341A1C5}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{C74E83AA-AE6D-4DEE-BA07-1379F47E07C0}" name="JSON_Variable" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{CEB535A9-8413-483C-A39B-7B0398A2BDB0}" name="Description" dataDxfId="2"/>
@@ -2617,7 +2562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA2D76F-1035-463A-85FC-3C41D6CE557B}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="B11" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2947,7 +2892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290A4E70-30C6-4246-8F18-09820CE6780F}">
   <dimension ref="A1:AG82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4133,10 +4078,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAE12B1-48D0-4CF3-91AC-FF4954E87BB4}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4235,95 +4180,95 @@
         <v>251</v>
       </c>
       <c r="C8" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C9" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" t="s">
         <v>255</v>
-      </c>
-      <c r="C10" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B11" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C11" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C12" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C13" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B15" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C15" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C16" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4334,51 +4279,51 @@
         <v>271</v>
       </c>
       <c r="C17" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>272</v>
+      </c>
+      <c r="B18" t="s">
         <v>273</v>
       </c>
-      <c r="B18" t="s">
-        <v>274</v>
-      </c>
       <c r="C18" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B19" t="s">
         <v>275</v>
       </c>
-      <c r="B19" t="s">
-        <v>276</v>
-      </c>
       <c r="C19" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>276</v>
+      </c>
+      <c r="B20" t="s">
         <v>277</v>
       </c>
-      <c r="B20" t="s">
-        <v>278</v>
-      </c>
       <c r="C20" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>278</v>
+      </c>
+      <c r="B21" t="s">
         <v>279</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>280</v>
-      </c>
-      <c r="C21" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4389,7 +4334,7 @@
         <v>282</v>
       </c>
       <c r="C22" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -4400,7 +4345,7 @@
         <v>284</v>
       </c>
       <c r="C23" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4411,7 +4356,7 @@
         <v>286</v>
       </c>
       <c r="C24" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -4422,7 +4367,7 @@
         <v>288</v>
       </c>
       <c r="C25" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4433,7 +4378,7 @@
         <v>290</v>
       </c>
       <c r="C26" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -4444,29 +4389,29 @@
         <v>292</v>
       </c>
       <c r="C27" t="s">
-        <v>272</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B28" t="s">
+        <v>295</v>
+      </c>
+      <c r="C28" t="s">
         <v>293</v>
-      </c>
-      <c r="B28" t="s">
-        <v>294</v>
-      </c>
-      <c r="C28" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B29" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C29" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -4477,7 +4422,7 @@
         <v>299</v>
       </c>
       <c r="C30" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -4488,7 +4433,7 @@
         <v>301</v>
       </c>
       <c r="C31" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4499,7 +4444,7 @@
         <v>303</v>
       </c>
       <c r="C32" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -4510,7 +4455,7 @@
         <v>305</v>
       </c>
       <c r="C33" t="s">
-        <v>297</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -4521,7 +4466,7 @@
         <v>307</v>
       </c>
       <c r="C34" t="s">
-        <v>297</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -4532,70 +4477,70 @@
         <v>309</v>
       </c>
       <c r="C35" t="s">
-        <v>310</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
+        <v>310</v>
+      </c>
+      <c r="B36" t="s">
         <v>311</v>
       </c>
-      <c r="B36" t="s">
-        <v>312</v>
-      </c>
       <c r="C36" t="s">
-        <v>310</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
+        <v>312</v>
+      </c>
+      <c r="B37" t="s">
         <v>313</v>
       </c>
-      <c r="B37" t="s">
-        <v>314</v>
-      </c>
       <c r="C37" t="s">
-        <v>310</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
+        <v>314</v>
+      </c>
+      <c r="B38" t="s">
         <v>315</v>
       </c>
-      <c r="B38" t="s">
-        <v>316</v>
-      </c>
       <c r="C38" t="s">
-        <v>310</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
+        <v>316</v>
+      </c>
+      <c r="B39" t="s">
         <v>317</v>
       </c>
-      <c r="B39" t="s">
-        <v>318</v>
-      </c>
       <c r="C39" t="s">
-        <v>310</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B40" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C40" t="s">
-        <v>310</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B41" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C41" t="s">
         <v>107</v>
@@ -4603,10 +4548,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B42" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C42" t="s">
         <v>107</v>
@@ -4614,10 +4559,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B43" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C43" t="s">
         <v>107</v>
@@ -4625,21 +4570,24 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>327</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="C44" t="s">
         <v>107</v>
       </c>
+      <c r="D44" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B45" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="C45" t="s">
         <v>107</v>
@@ -4647,10 +4595,10 @@
     </row>
     <row r="46" spans="1:4" s="6" customFormat="1">
       <c r="A46" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="B46" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C46" t="s">
         <v>107</v>
@@ -4659,10 +4607,10 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B47" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C47" t="s">
         <v>107</v>
@@ -4670,181 +4618,90 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
+        <v>327</v>
+      </c>
+      <c r="B48" t="s">
+        <v>328</v>
+      </c>
+      <c r="C48" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>330</v>
+      </c>
+      <c r="B49" t="s">
+        <v>331</v>
+      </c>
+      <c r="C49" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>332</v>
+      </c>
+      <c r="B50" t="s">
+        <v>333</v>
+      </c>
+      <c r="C50" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>334</v>
+      </c>
+      <c r="B51" t="s">
         <v>335</v>
       </c>
-      <c r="B48" t="s">
-        <v>334</v>
-      </c>
-      <c r="C48" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
+      <c r="C51" t="s">
         <v>336</v>
       </c>
-      <c r="B49" t="s">
-        <v>334</v>
-      </c>
-      <c r="C49" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
         <v>337</v>
       </c>
-      <c r="B50" t="s">
-        <v>334</v>
-      </c>
-      <c r="C50" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
+      <c r="B52" t="s">
         <v>338</v>
       </c>
-      <c r="B51" t="s">
-        <v>334</v>
-      </c>
-      <c r="C51" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" t="s">
-        <v>334</v>
-      </c>
       <c r="C52" t="s">
-        <v>107</v>
-      </c>
-      <c r="D52" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>340</v>
       </c>
       <c r="B53" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B54" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B55" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C55" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>344</v>
-      </c>
-      <c r="B56" t="s">
-        <v>345</v>
-      </c>
-      <c r="C56" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>347</v>
-      </c>
-      <c r="B57" t="s">
-        <v>348</v>
-      </c>
-      <c r="C57" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>349</v>
-      </c>
-      <c r="B58" t="s">
-        <v>350</v>
-      </c>
-      <c r="C58" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>351</v>
-      </c>
-      <c r="B59" t="s">
-        <v>352</v>
-      </c>
-      <c r="C59" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>354</v>
-      </c>
-      <c r="B60" t="s">
-        <v>355</v>
-      </c>
-      <c r="C60" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>357</v>
-      </c>
-      <c r="B61" t="s">
-        <v>358</v>
-      </c>
-      <c r="C61" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>359</v>
-      </c>
-      <c r="B62" t="s">
-        <v>360</v>
-      </c>
-      <c r="C62" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>361</v>
-      </c>
-      <c r="B63" t="s">
-        <v>362</v>
-      </c>
-      <c r="C63" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -4859,7 +4716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3029DAA5-5182-4BEE-B91D-DC72127632BA}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4896,15 +4753,15 @@
         <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="17" t="s">
-        <v>364</v>
+        <v>347</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4912,15 +4769,15 @@
         <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>365</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="17" t="s">
-        <v>366</v>
+        <v>349</v>
       </c>
       <c r="B6" t="s">
-        <v>367</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4928,199 +4785,199 @@
         <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>368</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="17" t="s">
-        <v>369</v>
+        <v>352</v>
       </c>
       <c r="B8" t="s">
-        <v>370</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="17" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
       <c r="B9" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="17" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="B10" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="17" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="B11" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="17" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="B12" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="17" t="s">
-        <v>379</v>
+        <v>362</v>
       </c>
       <c r="B13" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="17" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="B14" t="s">
-        <v>382</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="17" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="B15" t="s">
-        <v>384</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="17" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="B16" t="s">
-        <v>386</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="17" t="s">
-        <v>387</v>
+        <v>370</v>
       </c>
       <c r="B17" t="s">
-        <v>388</v>
+        <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="17" t="s">
-        <v>389</v>
+        <v>372</v>
       </c>
       <c r="B18" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="17" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="B19" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="17" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="B20" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="17" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="B21" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="17" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="B22" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="17" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
       <c r="B23" t="s">
-        <v>400</v>
+        <v>383</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="17" t="s">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="B24" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="17" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="B25" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="115.2">
       <c r="A26" s="17" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="72">
       <c r="A27" s="17" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="115.2">
       <c r="A28" s="17" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="72">
       <c r="A29" s="17" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="115.2">
       <c r="A30" s="17" t="s">
-        <v>413</v>
+        <v>396</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="72">
       <c r="A31" s="17" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>416</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>